<commit_message>
commit fixing product embedding update
</commit_message>
<xml_diff>
--- a/test-productknowledge.xlsx
+++ b/test-productknowledge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\divine\1agent\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\divine\1agent_openai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232538D2-A479-4255-BBD7-4F8AB042D590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53131BC-5F6D-433C-B66B-6871569C1244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E8E17BE-7925-433A-9232-1197F92B97E3}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{7E8E17BE-7925-433A-9232-1197F92B97E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>Makanan bergizi terbuat dari ayam yang dibakar</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +569,7 @@
         <v>25000</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>